<commit_message>
Se comenzó la parte de las gráficas
</commit_message>
<xml_diff>
--- a/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
+++ b/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTO_SCRUM_IS_II\LoboServicesFCC\Base de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B5DFFA-CC42-488D-ADA7-187C0983E6BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D8253B-5B05-4122-A80C-EA7FD9083CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="semestral" sheetId="6" r:id="rId1"/>
-    <sheet name="cargarmaterias" sheetId="14" r:id="rId2"/>
+    <sheet name="maestro(admin)" sheetId="14" r:id="rId2"/>
     <sheet name="materias" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3611" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3616" uniqueCount="1271">
   <si>
     <t>BENEMÉRITA UNIVERSIDAD AUTÓNOMA DE PUEBLA</t>
   </si>
@@ -3842,6 +3842,15 @@
   </si>
   <si>
     <t>Introducción a los Compiladores</t>
+  </si>
+  <si>
+    <t>matricula</t>
+  </si>
+  <si>
+    <t>contrasena</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -4760,7 +4769,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D1181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1110" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A1122" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F1154" sqref="F1154"/>
     </sheetView>
   </sheetViews>
@@ -21277,14 +21286,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82DFC6E-E826-4178-AF7A-7971C314C365}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21293,7 +21325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03379B5D-3AFA-44CA-B431-D65A6289F440}">
   <dimension ref="B2:J75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A61" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se ha terminado el Sprint III
</commit_message>
<xml_diff>
--- a/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
+++ b/Base de Datos/COMPUTACIÓN 201835  Semestral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROYECTO_SCRUM_IS_II\LoboServicesFCC\Base de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D8253B-5B05-4122-A80C-EA7FD9083CBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C573F-8E59-4221-9034-2158616B3B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="semestral" sheetId="6" r:id="rId1"/>
@@ -21288,7 +21288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82DFC6E-E826-4178-AF7A-7971C314C365}">
   <dimension ref="B2:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -21325,8 +21325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03379B5D-3AFA-44CA-B431-D65A6289F440}">
   <dimension ref="B2:J75"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22970,7 +22970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B65" s="2">
         <v>63</v>
       </c>
@@ -22989,8 +22989,14 @@
       <c r="G65" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I65" s="2">
+        <v>42</v>
+      </c>
+      <c r="J65" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B66" s="2">
         <v>64</v>
       </c>
@@ -23009,8 +23015,14 @@
       <c r="G66" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I66" s="2">
+        <v>56</v>
+      </c>
+      <c r="J66" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B67" s="2">
         <v>65</v>
       </c>
@@ -23029,8 +23041,14 @@
       <c r="G67" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I67" s="2">
+        <v>5</v>
+      </c>
+      <c r="J67" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B68" s="2">
         <v>66</v>
       </c>
@@ -23050,7 +23068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B69" s="2">
         <v>67</v>
       </c>
@@ -23070,7 +23088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B70" s="2">
         <v>68</v>
       </c>
@@ -23090,7 +23108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B71" s="2">
         <v>69</v>
       </c>
@@ -23110,7 +23128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B72" s="2">
         <v>70</v>
       </c>
@@ -23130,7 +23148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B73" s="2">
         <v>71</v>
       </c>
@@ -23150,7 +23168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B74" s="2">
         <v>72</v>
       </c>
@@ -23170,7 +23188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B75" s="2">
         <v>73</v>
       </c>

</xml_diff>